<commit_message>
fix: Default dictionary parsing.
</commit_message>
<xml_diff>
--- a/data/DynamicWorksheet.xlsx
+++ b/data/DynamicWorksheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>UID</t>
   </si>
@@ -98,18 +98,6 @@
   </si>
   <si>
     <t>b</t>
-  </si>
-  <si>
-    <t>bar</t>
-  </si>
-  <si>
-    <t>200, bar,false</t>
-  </si>
-  <si>
-    <t>2,foo|7</t>
-  </si>
-  <si>
-    <t>1001/1,bar</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1065,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5"/>
@@ -1238,21 +1226,11 @@
       <c r="E6" s="3">
         <v>0.1</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>